<commit_message>
update for unit cols fix
</commit_message>
<xml_diff>
--- a/projects/EcoFoci/dy2209/data/dy2209_faire.xlsx
+++ b/projects/EcoFoci/dy2209/data/dy2209_faire.xlsx
@@ -9917,10 +9917,10 @@
         </is>
       </c>
       <c r="J4" s="2" t="n">
-        <v>-163.8995</v>
+        <v>-163.06616</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>64.0038333333333</v>
+        <v>64.00383333333333</v>
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
@@ -10220,10 +10220,10 @@
         </is>
       </c>
       <c r="BU4" s="2" t="n">
-        <v>32.251</v>
+        <v>32</v>
       </c>
       <c r="BV4" s="2" t="n">
-        <v/>
+        <v>33</v>
       </c>
       <c r="BW4" s="2" t="n">
         <v>18</v>
@@ -10297,7 +10297,7 @@
       </c>
       <c r="CM4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN4" s="2" t="inlineStr">
@@ -10307,7 +10307,7 @@
       </c>
       <c r="CO4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP4" s="2" t="inlineStr">
@@ -10317,7 +10317,7 @@
       </c>
       <c r="CQ4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR4" s="2" t="inlineStr">
@@ -10327,7 +10327,7 @@
       </c>
       <c r="CS4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT4" s="2" t="n">
@@ -10345,7 +10345,7 @@
       </c>
       <c r="CW4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX4" s="2" t="inlineStr">
@@ -10355,7 +10355,7 @@
       </c>
       <c r="CY4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ4" s="2" t="inlineStr">
@@ -10365,7 +10365,7 @@
       </c>
       <c r="DA4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB4" s="2" t="inlineStr">
@@ -10375,7 +10375,7 @@
       </c>
       <c r="DC4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD4" s="2" t="inlineStr">
@@ -10385,7 +10385,7 @@
       </c>
       <c r="DE4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF4" s="2" t="inlineStr">
@@ -10400,7 +10400,7 @@
       </c>
       <c r="DH4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI4" s="2" t="inlineStr">
@@ -10415,7 +10415,7 @@
       </c>
       <c r="DK4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL4" s="2" t="inlineStr">
@@ -10425,7 +10425,7 @@
       </c>
       <c r="DM4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN4" s="2" t="inlineStr">
@@ -10435,7 +10435,7 @@
       </c>
       <c r="DO4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP4" s="2" t="inlineStr">
@@ -10445,7 +10445,7 @@
       </c>
       <c r="DQ4" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR4" s="2" t="inlineStr">
@@ -10455,7 +10455,7 @@
       </c>
       <c r="DS4" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT4" s="2" t="inlineStr">
@@ -10465,7 +10465,7 @@
       </c>
       <c r="DU4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV4" s="2" t="inlineStr">
@@ -10475,7 +10475,7 @@
       </c>
       <c r="DW4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX4" s="2" t="inlineStr">
@@ -10485,7 +10485,7 @@
       </c>
       <c r="DY4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ4" s="2" t="inlineStr">
@@ -10495,17 +10495,17 @@
       </c>
       <c r="EA4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB4" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED4" s="2" t="inlineStr">
@@ -10515,7 +10515,7 @@
       </c>
       <c r="EE4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF4" s="2" t="inlineStr">
@@ -10530,7 +10530,7 @@
       </c>
       <c r="EH4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI4" s="2" t="inlineStr">
@@ -10545,7 +10545,7 @@
       </c>
       <c r="EK4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL4" s="2" t="inlineStr">
@@ -10555,7 +10555,7 @@
       </c>
       <c r="EM4" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN4" s="2" t="n">
@@ -10573,7 +10573,7 @@
       </c>
       <c r="EQ4" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER4" s="2" t="inlineStr">
@@ -10583,7 +10583,7 @@
       </c>
       <c r="ES4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET4" s="2" t="inlineStr">
@@ -10593,7 +10593,7 @@
       </c>
       <c r="EU4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV4" s="2" t="inlineStr">
@@ -10620,22 +10620,24 @@
       <c r="FA4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="FB4" s="2" t="n">
-        <v/>
+      <c r="FB4" s="2" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE4" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF4" s="2" t="n">
@@ -10652,7 +10654,7 @@
         </is>
       </c>
       <c r="FI4" s="2" t="n">
-        <v/>
+        <v>0.716</v>
       </c>
       <c r="FJ4" s="2" t="inlineStr">
         <is>
@@ -10730,22 +10732,22 @@
       </c>
       <c r="FZ4" t="inlineStr">
         <is>
-          <t>degree Celsius</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA4" t="inlineStr">
         <is>
-          <t>µmol s-1 m-2</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB4" t="inlineStr">
         <is>
-          <t>mb</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC4" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -10796,10 +10798,10 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>-163.8995</v>
+        <v>-163.06616</v>
       </c>
       <c r="K5" t="n">
-        <v>64.0038333333333</v>
+        <v>64.00383333333333</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -11099,10 +11101,10 @@
         </is>
       </c>
       <c r="BU5" t="n">
-        <v>19.521</v>
+        <v>19.4</v>
       </c>
       <c r="BV5" t="n">
-        <v/>
+        <v>20.4</v>
       </c>
       <c r="BW5" t="n">
         <v>18</v>
@@ -11176,7 +11178,7 @@
       </c>
       <c r="CM5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN5" t="inlineStr">
@@ -11186,7 +11188,7 @@
       </c>
       <c r="CO5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP5" t="inlineStr">
@@ -11196,7 +11198,7 @@
       </c>
       <c r="CQ5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR5" t="inlineStr">
@@ -11206,7 +11208,7 @@
       </c>
       <c r="CS5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT5" t="n">
@@ -11224,7 +11226,7 @@
       </c>
       <c r="CW5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX5" t="inlineStr">
@@ -11234,7 +11236,7 @@
       </c>
       <c r="CY5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ5" t="inlineStr">
@@ -11244,7 +11246,7 @@
       </c>
       <c r="DA5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB5" t="inlineStr">
@@ -11254,7 +11256,7 @@
       </c>
       <c r="DC5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD5" t="inlineStr">
@@ -11264,7 +11266,7 @@
       </c>
       <c r="DE5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF5" t="inlineStr">
@@ -11279,7 +11281,7 @@
       </c>
       <c r="DH5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI5" t="inlineStr">
@@ -11294,7 +11296,7 @@
       </c>
       <c r="DK5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL5" t="inlineStr">
@@ -11304,7 +11306,7 @@
       </c>
       <c r="DM5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN5" t="inlineStr">
@@ -11314,7 +11316,7 @@
       </c>
       <c r="DO5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP5" t="inlineStr">
@@ -11324,7 +11326,7 @@
       </c>
       <c r="DQ5" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR5" t="inlineStr">
@@ -11334,7 +11336,7 @@
       </c>
       <c r="DS5" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT5" t="inlineStr">
@@ -11344,7 +11346,7 @@
       </c>
       <c r="DU5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV5" t="inlineStr">
@@ -11354,7 +11356,7 @@
       </c>
       <c r="DW5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX5" t="inlineStr">
@@ -11364,7 +11366,7 @@
       </c>
       <c r="DY5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ5" t="inlineStr">
@@ -11374,17 +11376,17 @@
       </c>
       <c r="EA5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB5" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED5" t="inlineStr">
@@ -11394,7 +11396,7 @@
       </c>
       <c r="EE5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF5" t="inlineStr">
@@ -11409,7 +11411,7 @@
       </c>
       <c r="EH5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI5" t="inlineStr">
@@ -11424,7 +11426,7 @@
       </c>
       <c r="EK5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL5" t="inlineStr">
@@ -11434,7 +11436,7 @@
       </c>
       <c r="EM5" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN5" t="n">
@@ -11452,7 +11454,7 @@
       </c>
       <c r="EQ5" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER5" t="inlineStr">
@@ -11462,7 +11464,7 @@
       </c>
       <c r="ES5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET5" t="inlineStr">
@@ -11472,7 +11474,7 @@
       </c>
       <c r="EU5" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV5" t="inlineStr">
@@ -11499,22 +11501,24 @@
       <c r="FA5" t="n">
         <v>1</v>
       </c>
-      <c r="FB5" t="n">
-        <v/>
+      <c r="FB5" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC5" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD5" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE5" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF5" t="n">
@@ -11531,7 +11535,7 @@
         </is>
       </c>
       <c r="FI5" t="n">
-        <v/>
+        <v>0.535</v>
       </c>
       <c r="FJ5" t="inlineStr">
         <is>
@@ -11609,22 +11613,22 @@
       </c>
       <c r="FZ5" t="inlineStr">
         <is>
-          <t>degree Celsius</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA5" t="inlineStr">
         <is>
-          <t>µmol s-1 m-2</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB5" t="inlineStr">
         <is>
-          <t>mb</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC5" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -11675,10 +11679,10 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>-163.8995</v>
+        <v>-163.06616</v>
       </c>
       <c r="K6" t="n">
-        <v>64.0038333333333</v>
+        <v>64.00383333333333</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -11978,10 +11982,10 @@
         </is>
       </c>
       <c r="BU6" t="n">
-        <v>8.801</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="BV6" t="n">
-        <v/>
+        <v>9.699999999999999</v>
       </c>
       <c r="BW6" t="n">
         <v>18</v>
@@ -12055,7 +12059,7 @@
       </c>
       <c r="CM6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN6" t="inlineStr">
@@ -12065,7 +12069,7 @@
       </c>
       <c r="CO6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP6" t="inlineStr">
@@ -12075,7 +12079,7 @@
       </c>
       <c r="CQ6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR6" t="inlineStr">
@@ -12085,7 +12089,7 @@
       </c>
       <c r="CS6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT6" t="n">
@@ -12103,7 +12107,7 @@
       </c>
       <c r="CW6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX6" t="inlineStr">
@@ -12113,7 +12117,7 @@
       </c>
       <c r="CY6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ6" t="inlineStr">
@@ -12123,7 +12127,7 @@
       </c>
       <c r="DA6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB6" t="inlineStr">
@@ -12133,7 +12137,7 @@
       </c>
       <c r="DC6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD6" t="inlineStr">
@@ -12143,7 +12147,7 @@
       </c>
       <c r="DE6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF6" t="inlineStr">
@@ -12158,7 +12162,7 @@
       </c>
       <c r="DH6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI6" t="inlineStr">
@@ -12173,7 +12177,7 @@
       </c>
       <c r="DK6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL6" t="inlineStr">
@@ -12183,7 +12187,7 @@
       </c>
       <c r="DM6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN6" t="inlineStr">
@@ -12193,7 +12197,7 @@
       </c>
       <c r="DO6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP6" t="inlineStr">
@@ -12203,7 +12207,7 @@
       </c>
       <c r="DQ6" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR6" t="inlineStr">
@@ -12213,7 +12217,7 @@
       </c>
       <c r="DS6" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT6" t="inlineStr">
@@ -12223,7 +12227,7 @@
       </c>
       <c r="DU6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV6" t="inlineStr">
@@ -12233,7 +12237,7 @@
       </c>
       <c r="DW6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX6" t="inlineStr">
@@ -12243,7 +12247,7 @@
       </c>
       <c r="DY6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ6" t="inlineStr">
@@ -12253,17 +12257,17 @@
       </c>
       <c r="EA6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB6" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED6" t="inlineStr">
@@ -12273,7 +12277,7 @@
       </c>
       <c r="EE6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF6" t="inlineStr">
@@ -12288,7 +12292,7 @@
       </c>
       <c r="EH6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI6" t="inlineStr">
@@ -12303,7 +12307,7 @@
       </c>
       <c r="EK6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL6" t="inlineStr">
@@ -12313,7 +12317,7 @@
       </c>
       <c r="EM6" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN6" t="n">
@@ -12331,7 +12335,7 @@
       </c>
       <c r="EQ6" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER6" t="inlineStr">
@@ -12341,7 +12345,7 @@
       </c>
       <c r="ES6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET6" t="inlineStr">
@@ -12351,7 +12355,7 @@
       </c>
       <c r="EU6" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV6" t="inlineStr">
@@ -12378,22 +12382,24 @@
       <c r="FA6" t="n">
         <v>1</v>
       </c>
-      <c r="FB6" t="n">
-        <v/>
+      <c r="FB6" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC6" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD6" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE6" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF6" t="n">
@@ -12410,7 +12416,7 @@
         </is>
       </c>
       <c r="FI6" t="n">
-        <v/>
+        <v>1</v>
       </c>
       <c r="FJ6" t="inlineStr">
         <is>
@@ -12488,22 +12494,22 @@
       </c>
       <c r="FZ6" t="inlineStr">
         <is>
-          <t>degree Celsius</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA6" t="inlineStr">
         <is>
-          <t>µmol s-1 m-2</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB6" t="inlineStr">
         <is>
-          <t>mb</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC6" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -12554,10 +12560,10 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>-168.218333333333</v>
+        <v>-168.21834</v>
       </c>
       <c r="K7" t="n">
-        <v>64.6733333333333</v>
+        <v>64.67333333333333</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -12857,10 +12863,10 @@
         </is>
       </c>
       <c r="BU7" t="n">
-        <v>32.889</v>
+        <v>32.7</v>
       </c>
       <c r="BV7" t="n">
-        <v/>
+        <v>33.7</v>
       </c>
       <c r="BW7" t="n">
         <v>37</v>
@@ -12934,7 +12940,7 @@
       </c>
       <c r="CM7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN7" t="inlineStr">
@@ -12944,7 +12950,7 @@
       </c>
       <c r="CO7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP7" t="inlineStr">
@@ -12954,7 +12960,7 @@
       </c>
       <c r="CQ7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR7" t="inlineStr">
@@ -12964,7 +12970,7 @@
       </c>
       <c r="CS7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT7" t="n">
@@ -12982,7 +12988,7 @@
       </c>
       <c r="CW7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX7" t="inlineStr">
@@ -12992,7 +12998,7 @@
       </c>
       <c r="CY7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ7" t="inlineStr">
@@ -13002,7 +13008,7 @@
       </c>
       <c r="DA7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB7" t="inlineStr">
@@ -13012,7 +13018,7 @@
       </c>
       <c r="DC7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD7" t="inlineStr">
@@ -13022,7 +13028,7 @@
       </c>
       <c r="DE7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF7" t="inlineStr">
@@ -13037,7 +13043,7 @@
       </c>
       <c r="DH7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI7" t="inlineStr">
@@ -13052,7 +13058,7 @@
       </c>
       <c r="DK7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL7" t="inlineStr">
@@ -13062,7 +13068,7 @@
       </c>
       <c r="DM7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN7" t="inlineStr">
@@ -13072,7 +13078,7 @@
       </c>
       <c r="DO7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP7" t="inlineStr">
@@ -13082,7 +13088,7 @@
       </c>
       <c r="DQ7" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR7" t="inlineStr">
@@ -13092,7 +13098,7 @@
       </c>
       <c r="DS7" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT7" t="inlineStr">
@@ -13102,7 +13108,7 @@
       </c>
       <c r="DU7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV7" t="inlineStr">
@@ -13112,7 +13118,7 @@
       </c>
       <c r="DW7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX7" t="inlineStr">
@@ -13122,7 +13128,7 @@
       </c>
       <c r="DY7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ7" t="inlineStr">
@@ -13132,17 +13138,17 @@
       </c>
       <c r="EA7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB7" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED7" t="inlineStr">
@@ -13152,7 +13158,7 @@
       </c>
       <c r="EE7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF7" t="inlineStr">
@@ -13167,7 +13173,7 @@
       </c>
       <c r="EH7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI7" t="inlineStr">
@@ -13182,7 +13188,7 @@
       </c>
       <c r="EK7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL7" t="inlineStr">
@@ -13192,7 +13198,7 @@
       </c>
       <c r="EM7" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN7" t="n">
@@ -13210,7 +13216,7 @@
       </c>
       <c r="EQ7" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER7" t="inlineStr">
@@ -13220,7 +13226,7 @@
       </c>
       <c r="ES7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET7" t="inlineStr">
@@ -13230,7 +13236,7 @@
       </c>
       <c r="EU7" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV7" t="inlineStr">
@@ -13257,22 +13263,24 @@
       <c r="FA7" t="n">
         <v>1</v>
       </c>
-      <c r="FB7" t="n">
-        <v/>
+      <c r="FB7" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC7" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD7" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE7" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF7" t="n">
@@ -13289,7 +13297,7 @@
         </is>
       </c>
       <c r="FI7" t="n">
-        <v/>
+        <v>1.33</v>
       </c>
       <c r="FJ7" t="inlineStr">
         <is>
@@ -13367,22 +13375,22 @@
       </c>
       <c r="FZ7" t="inlineStr">
         <is>
-          <t>degree Celsius</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA7" t="inlineStr">
         <is>
-          <t>µmol s-1 m-2</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB7" t="inlineStr">
         <is>
-          <t>mb</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC7" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -13433,10 +13441,10 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>-168.218333333333</v>
+        <v>-168.21834</v>
       </c>
       <c r="K8" t="n">
-        <v>64.6733333333333</v>
+        <v>64.67333333333333</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -13736,10 +13744,10 @@
         </is>
       </c>
       <c r="BU8" t="n">
-        <v>18.886</v>
+        <v>18.8</v>
       </c>
       <c r="BV8" t="n">
-        <v/>
+        <v>19.8</v>
       </c>
       <c r="BW8" t="n">
         <v>37</v>
@@ -13813,7 +13821,7 @@
       </c>
       <c r="CM8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN8" t="inlineStr">
@@ -13823,7 +13831,7 @@
       </c>
       <c r="CO8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP8" t="inlineStr">
@@ -13833,7 +13841,7 @@
       </c>
       <c r="CQ8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR8" t="inlineStr">
@@ -13843,7 +13851,7 @@
       </c>
       <c r="CS8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT8" t="n">
@@ -13861,7 +13869,7 @@
       </c>
       <c r="CW8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX8" t="inlineStr">
@@ -13871,7 +13879,7 @@
       </c>
       <c r="CY8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ8" t="inlineStr">
@@ -13881,7 +13889,7 @@
       </c>
       <c r="DA8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB8" t="inlineStr">
@@ -13891,7 +13899,7 @@
       </c>
       <c r="DC8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD8" t="inlineStr">
@@ -13901,7 +13909,7 @@
       </c>
       <c r="DE8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF8" t="inlineStr">
@@ -13916,7 +13924,7 @@
       </c>
       <c r="DH8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI8" t="inlineStr">
@@ -13931,7 +13939,7 @@
       </c>
       <c r="DK8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL8" t="inlineStr">
@@ -13941,7 +13949,7 @@
       </c>
       <c r="DM8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN8" t="inlineStr">
@@ -13951,7 +13959,7 @@
       </c>
       <c r="DO8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP8" t="inlineStr">
@@ -13961,7 +13969,7 @@
       </c>
       <c r="DQ8" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR8" t="inlineStr">
@@ -13971,7 +13979,7 @@
       </c>
       <c r="DS8" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT8" t="inlineStr">
@@ -13981,7 +13989,7 @@
       </c>
       <c r="DU8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV8" t="inlineStr">
@@ -13991,7 +13999,7 @@
       </c>
       <c r="DW8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX8" t="inlineStr">
@@ -14001,7 +14009,7 @@
       </c>
       <c r="DY8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ8" t="inlineStr">
@@ -14011,17 +14019,17 @@
       </c>
       <c r="EA8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB8" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED8" t="inlineStr">
@@ -14031,7 +14039,7 @@
       </c>
       <c r="EE8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF8" t="inlineStr">
@@ -14046,7 +14054,7 @@
       </c>
       <c r="EH8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI8" t="inlineStr">
@@ -14061,7 +14069,7 @@
       </c>
       <c r="EK8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL8" t="inlineStr">
@@ -14071,7 +14079,7 @@
       </c>
       <c r="EM8" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN8" t="n">
@@ -14089,7 +14097,7 @@
       </c>
       <c r="EQ8" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER8" t="inlineStr">
@@ -14099,7 +14107,7 @@
       </c>
       <c r="ES8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET8" t="inlineStr">
@@ -14109,7 +14117,7 @@
       </c>
       <c r="EU8" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV8" t="inlineStr">
@@ -14136,22 +14144,24 @@
       <c r="FA8" t="n">
         <v>1</v>
       </c>
-      <c r="FB8" t="n">
-        <v/>
+      <c r="FB8" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC8" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD8" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE8" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF8" t="n">
@@ -14168,7 +14178,7 @@
         </is>
       </c>
       <c r="FI8" t="n">
-        <v/>
+        <v>1.43</v>
       </c>
       <c r="FJ8" t="inlineStr">
         <is>
@@ -14246,22 +14256,22 @@
       </c>
       <c r="FZ8" t="inlineStr">
         <is>
-          <t>degree Celsius</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA8" t="inlineStr">
         <is>
-          <t>µmol s-1 m-2</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB8" t="inlineStr">
         <is>
-          <t>mb</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC8" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -14312,10 +14322,10 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>-168.218333333333</v>
+        <v>-168.21834</v>
       </c>
       <c r="K9" t="n">
-        <v>64.6733333333333</v>
+        <v>64.67333333333333</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -14615,10 +14625,10 @@
         </is>
       </c>
       <c r="BU9" t="n">
-        <v>8.337999999999999</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="BV9" t="n">
-        <v/>
+        <v>9.300000000000001</v>
       </c>
       <c r="BW9" t="n">
         <v>37</v>
@@ -14692,7 +14702,7 @@
       </c>
       <c r="CM9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN9" t="inlineStr">
@@ -14702,7 +14712,7 @@
       </c>
       <c r="CO9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP9" t="inlineStr">
@@ -14712,7 +14722,7 @@
       </c>
       <c r="CQ9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR9" t="inlineStr">
@@ -14722,7 +14732,7 @@
       </c>
       <c r="CS9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT9" t="n">
@@ -14740,7 +14750,7 @@
       </c>
       <c r="CW9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX9" t="inlineStr">
@@ -14750,7 +14760,7 @@
       </c>
       <c r="CY9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ9" t="inlineStr">
@@ -14760,7 +14770,7 @@
       </c>
       <c r="DA9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB9" t="inlineStr">
@@ -14770,7 +14780,7 @@
       </c>
       <c r="DC9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD9" t="inlineStr">
@@ -14780,7 +14790,7 @@
       </c>
       <c r="DE9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF9" t="inlineStr">
@@ -14795,7 +14805,7 @@
       </c>
       <c r="DH9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI9" t="inlineStr">
@@ -14810,7 +14820,7 @@
       </c>
       <c r="DK9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL9" t="inlineStr">
@@ -14820,7 +14830,7 @@
       </c>
       <c r="DM9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN9" t="inlineStr">
@@ -14830,7 +14840,7 @@
       </c>
       <c r="DO9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP9" t="inlineStr">
@@ -14840,7 +14850,7 @@
       </c>
       <c r="DQ9" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR9" t="inlineStr">
@@ -14850,7 +14860,7 @@
       </c>
       <c r="DS9" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT9" t="inlineStr">
@@ -14860,7 +14870,7 @@
       </c>
       <c r="DU9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV9" t="inlineStr">
@@ -14870,7 +14880,7 @@
       </c>
       <c r="DW9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX9" t="inlineStr">
@@ -14880,7 +14890,7 @@
       </c>
       <c r="DY9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ9" t="inlineStr">
@@ -14890,17 +14900,17 @@
       </c>
       <c r="EA9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB9" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED9" t="inlineStr">
@@ -14910,7 +14920,7 @@
       </c>
       <c r="EE9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF9" t="inlineStr">
@@ -14925,7 +14935,7 @@
       </c>
       <c r="EH9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI9" t="inlineStr">
@@ -14940,7 +14950,7 @@
       </c>
       <c r="EK9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL9" t="inlineStr">
@@ -14950,7 +14960,7 @@
       </c>
       <c r="EM9" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN9" t="n">
@@ -14968,7 +14978,7 @@
       </c>
       <c r="EQ9" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER9" t="inlineStr">
@@ -14978,7 +14988,7 @@
       </c>
       <c r="ES9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET9" t="inlineStr">
@@ -14988,7 +14998,7 @@
       </c>
       <c r="EU9" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV9" t="inlineStr">
@@ -15015,22 +15025,24 @@
       <c r="FA9" t="n">
         <v>1</v>
       </c>
-      <c r="FB9" t="n">
-        <v/>
+      <c r="FB9" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC9" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD9" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE9" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF9" t="n">
@@ -15047,7 +15059,7 @@
         </is>
       </c>
       <c r="FI9" t="n">
-        <v/>
+        <v>1.12</v>
       </c>
       <c r="FJ9" t="inlineStr">
         <is>
@@ -15125,22 +15137,22 @@
       </c>
       <c r="FZ9" t="inlineStr">
         <is>
-          <t>degree Celsius</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA9" t="inlineStr">
         <is>
-          <t>µmol s-1 m-2</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB9" t="inlineStr">
         <is>
-          <t>mb</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC9" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -15194,7 +15206,7 @@
         <v>-169.1</v>
       </c>
       <c r="K10" t="n">
-        <v>64.6791666666667</v>
+        <v>64.67916666666666</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -15494,10 +15506,10 @@
         </is>
       </c>
       <c r="BU10" t="n">
-        <v>40.673</v>
+        <v>40.4</v>
       </c>
       <c r="BV10" t="n">
-        <v/>
+        <v>41.4</v>
       </c>
       <c r="BW10" t="n">
         <v>45</v>
@@ -15569,7 +15581,7 @@
       </c>
       <c r="CM10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN10" t="inlineStr">
@@ -15579,7 +15591,7 @@
       </c>
       <c r="CO10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP10" t="inlineStr">
@@ -15589,7 +15601,7 @@
       </c>
       <c r="CQ10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR10" t="inlineStr">
@@ -15599,7 +15611,7 @@
       </c>
       <c r="CS10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT10" t="n">
@@ -15617,7 +15629,7 @@
       </c>
       <c r="CW10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX10" t="inlineStr">
@@ -15627,7 +15639,7 @@
       </c>
       <c r="CY10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ10" t="inlineStr">
@@ -15637,7 +15649,7 @@
       </c>
       <c r="DA10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB10" t="inlineStr">
@@ -15647,7 +15659,7 @@
       </c>
       <c r="DC10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD10" t="inlineStr">
@@ -15657,7 +15669,7 @@
       </c>
       <c r="DE10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF10" t="inlineStr">
@@ -15672,7 +15684,7 @@
       </c>
       <c r="DH10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI10" t="inlineStr">
@@ -15687,7 +15699,7 @@
       </c>
       <c r="DK10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL10" t="inlineStr">
@@ -15697,7 +15709,7 @@
       </c>
       <c r="DM10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN10" t="inlineStr">
@@ -15707,7 +15719,7 @@
       </c>
       <c r="DO10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP10" t="inlineStr">
@@ -15717,7 +15729,7 @@
       </c>
       <c r="DQ10" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR10" t="inlineStr">
@@ -15727,7 +15739,7 @@
       </c>
       <c r="DS10" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT10" t="inlineStr">
@@ -15737,7 +15749,7 @@
       </c>
       <c r="DU10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV10" t="inlineStr">
@@ -15747,7 +15759,7 @@
       </c>
       <c r="DW10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX10" t="inlineStr">
@@ -15757,7 +15769,7 @@
       </c>
       <c r="DY10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ10" t="inlineStr">
@@ -15767,17 +15779,17 @@
       </c>
       <c r="EA10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB10" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED10" t="inlineStr">
@@ -15787,7 +15799,7 @@
       </c>
       <c r="EE10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF10" t="inlineStr">
@@ -15802,7 +15814,7 @@
       </c>
       <c r="EH10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI10" t="inlineStr">
@@ -15817,7 +15829,7 @@
       </c>
       <c r="EK10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL10" t="inlineStr">
@@ -15827,7 +15839,7 @@
       </c>
       <c r="EM10" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN10" t="n">
@@ -15845,7 +15857,7 @@
       </c>
       <c r="EQ10" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER10" t="inlineStr">
@@ -15855,7 +15867,7 @@
       </c>
       <c r="ES10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET10" t="inlineStr">
@@ -15865,7 +15877,7 @@
       </c>
       <c r="EU10" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV10" t="inlineStr">
@@ -15892,22 +15904,24 @@
       <c r="FA10" t="n">
         <v>1</v>
       </c>
-      <c r="FB10" t="n">
-        <v/>
+      <c r="FB10" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC10" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD10" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE10" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF10" t="n">
@@ -15924,7 +15938,7 @@
         </is>
       </c>
       <c r="FI10" t="n">
-        <v/>
+        <v>0.6830000000000001</v>
       </c>
       <c r="FJ10" t="inlineStr">
         <is>
@@ -16011,7 +16025,7 @@
       </c>
       <c r="GC10" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -16065,7 +16079,7 @@
         <v>-169.1</v>
       </c>
       <c r="K11" t="n">
-        <v>64.6791666666667</v>
+        <v>64.67916666666666</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -16365,10 +16379,10 @@
         </is>
       </c>
       <c r="BU11" t="n">
-        <v>28.728</v>
+        <v>28.5</v>
       </c>
       <c r="BV11" t="n">
-        <v/>
+        <v>29.5</v>
       </c>
       <c r="BW11" t="n">
         <v>45</v>
@@ -16440,7 +16454,7 @@
       </c>
       <c r="CM11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN11" t="inlineStr">
@@ -16450,7 +16464,7 @@
       </c>
       <c r="CO11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP11" t="inlineStr">
@@ -16460,7 +16474,7 @@
       </c>
       <c r="CQ11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR11" t="inlineStr">
@@ -16470,7 +16484,7 @@
       </c>
       <c r="CS11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT11" t="n">
@@ -16488,7 +16502,7 @@
       </c>
       <c r="CW11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX11" t="inlineStr">
@@ -16498,7 +16512,7 @@
       </c>
       <c r="CY11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ11" t="inlineStr">
@@ -16508,7 +16522,7 @@
       </c>
       <c r="DA11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB11" t="inlineStr">
@@ -16518,7 +16532,7 @@
       </c>
       <c r="DC11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD11" t="inlineStr">
@@ -16528,7 +16542,7 @@
       </c>
       <c r="DE11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF11" t="inlineStr">
@@ -16543,7 +16557,7 @@
       </c>
       <c r="DH11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI11" t="inlineStr">
@@ -16558,7 +16572,7 @@
       </c>
       <c r="DK11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL11" t="inlineStr">
@@ -16568,7 +16582,7 @@
       </c>
       <c r="DM11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN11" t="inlineStr">
@@ -16578,7 +16592,7 @@
       </c>
       <c r="DO11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP11" t="n">
@@ -16604,7 +16618,7 @@
       </c>
       <c r="DU11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV11" t="inlineStr">
@@ -16614,7 +16628,7 @@
       </c>
       <c r="DW11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX11" t="inlineStr">
@@ -16624,7 +16638,7 @@
       </c>
       <c r="DY11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ11" t="inlineStr">
@@ -16634,17 +16648,17 @@
       </c>
       <c r="EA11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
-        </is>
-      </c>
-      <c r="EB11" t="inlineStr">
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EB11" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="EC11" s="2" t="inlineStr">
         <is>
           <t>µmol/L</t>
         </is>
       </c>
-      <c r="EC11" s="2" t="n">
-        <v>0.86</v>
-      </c>
       <c r="ED11" t="inlineStr">
         <is>
           <t>missing: not collected</t>
@@ -16652,7 +16666,7 @@
       </c>
       <c r="EE11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF11" t="inlineStr">
@@ -16667,7 +16681,7 @@
       </c>
       <c r="EH11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI11" t="inlineStr">
@@ -16682,7 +16696,7 @@
       </c>
       <c r="EK11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL11" t="n">
@@ -16716,7 +16730,7 @@
       </c>
       <c r="ES11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET11" t="inlineStr">
@@ -16726,7 +16740,7 @@
       </c>
       <c r="EU11" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV11" t="inlineStr">
@@ -16753,22 +16767,24 @@
       <c r="FA11" t="n">
         <v>1</v>
       </c>
-      <c r="FB11" t="n">
-        <v/>
+      <c r="FB11" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC11" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD11" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE11" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF11" t="n">
@@ -16785,7 +16801,7 @@
         </is>
       </c>
       <c r="FI11" t="n">
-        <v/>
+        <v>2.6</v>
       </c>
       <c r="FJ11" t="inlineStr">
         <is>
@@ -16862,7 +16878,7 @@
       </c>
       <c r="GC11" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -16916,7 +16932,7 @@
         <v>-169.1</v>
       </c>
       <c r="K12" t="n">
-        <v>64.6791666666667</v>
+        <v>64.67916666666666</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -17216,10 +17232,10 @@
         </is>
       </c>
       <c r="BU12" t="n">
-        <v>8.394</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="BV12" t="n">
-        <v/>
+        <v>9.300000000000001</v>
       </c>
       <c r="BW12" t="n">
         <v>45</v>
@@ -17291,7 +17307,7 @@
       </c>
       <c r="CM12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN12" t="inlineStr">
@@ -17301,7 +17317,7 @@
       </c>
       <c r="CO12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP12" t="inlineStr">
@@ -17311,7 +17327,7 @@
       </c>
       <c r="CQ12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR12" t="inlineStr">
@@ -17321,7 +17337,7 @@
       </c>
       <c r="CS12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT12" t="n">
@@ -17339,7 +17355,7 @@
       </c>
       <c r="CW12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX12" t="inlineStr">
@@ -17349,7 +17365,7 @@
       </c>
       <c r="CY12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ12" t="inlineStr">
@@ -17359,7 +17375,7 @@
       </c>
       <c r="DA12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB12" t="inlineStr">
@@ -17369,7 +17385,7 @@
       </c>
       <c r="DC12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD12" t="inlineStr">
@@ -17379,7 +17395,7 @@
       </c>
       <c r="DE12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF12" t="inlineStr">
@@ -17394,7 +17410,7 @@
       </c>
       <c r="DH12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI12" t="inlineStr">
@@ -17409,7 +17425,7 @@
       </c>
       <c r="DK12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL12" t="inlineStr">
@@ -17419,7 +17435,7 @@
       </c>
       <c r="DM12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN12" t="inlineStr">
@@ -17429,7 +17445,7 @@
       </c>
       <c r="DO12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP12" t="inlineStr">
@@ -17439,7 +17455,7 @@
       </c>
       <c r="DQ12" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR12" t="inlineStr">
@@ -17449,7 +17465,7 @@
       </c>
       <c r="DS12" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT12" t="inlineStr">
@@ -17459,7 +17475,7 @@
       </c>
       <c r="DU12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV12" t="inlineStr">
@@ -17469,7 +17485,7 @@
       </c>
       <c r="DW12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX12" t="inlineStr">
@@ -17479,7 +17495,7 @@
       </c>
       <c r="DY12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ12" t="inlineStr">
@@ -17489,17 +17505,17 @@
       </c>
       <c r="EA12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB12" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED12" t="inlineStr">
@@ -17509,7 +17525,7 @@
       </c>
       <c r="EE12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF12" t="inlineStr">
@@ -17524,7 +17540,7 @@
       </c>
       <c r="EH12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI12" t="inlineStr">
@@ -17539,7 +17555,7 @@
       </c>
       <c r="EK12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL12" t="inlineStr">
@@ -17549,7 +17565,7 @@
       </c>
       <c r="EM12" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN12" t="n">
@@ -17567,7 +17583,7 @@
       </c>
       <c r="EQ12" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER12" t="inlineStr">
@@ -17577,7 +17593,7 @@
       </c>
       <c r="ES12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET12" t="inlineStr">
@@ -17587,7 +17603,7 @@
       </c>
       <c r="EU12" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV12" t="inlineStr">
@@ -17614,22 +17630,24 @@
       <c r="FA12" t="n">
         <v>1</v>
       </c>
-      <c r="FB12" t="n">
-        <v/>
+      <c r="FB12" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC12" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD12" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE12" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF12" t="n">
@@ -17646,7 +17664,7 @@
         </is>
       </c>
       <c r="FI12" t="n">
-        <v/>
+        <v>1.63</v>
       </c>
       <c r="FJ12" t="inlineStr">
         <is>
@@ -17723,7 +17741,7 @@
       </c>
       <c r="GC12" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -17774,10 +17792,10 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>-169.146333333333</v>
+        <v>-169.14633</v>
       </c>
       <c r="K13" t="n">
-        <v>64.1463333333333</v>
+        <v>64.9915</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -18075,10 +18093,10 @@
         </is>
       </c>
       <c r="BU13" t="n">
-        <v>42.571</v>
+        <v>42.3</v>
       </c>
       <c r="BV13" t="n">
-        <v/>
+        <v>43.3</v>
       </c>
       <c r="BW13" t="n">
         <v>48</v>
@@ -18152,7 +18170,7 @@
       </c>
       <c r="CM13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN13" t="inlineStr">
@@ -18162,7 +18180,7 @@
       </c>
       <c r="CO13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP13" t="inlineStr">
@@ -18172,7 +18190,7 @@
       </c>
       <c r="CQ13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR13" t="inlineStr">
@@ -18182,7 +18200,7 @@
       </c>
       <c r="CS13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT13" t="n">
@@ -18200,7 +18218,7 @@
       </c>
       <c r="CW13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX13" t="inlineStr">
@@ -18210,7 +18228,7 @@
       </c>
       <c r="CY13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ13" t="inlineStr">
@@ -18220,7 +18238,7 @@
       </c>
       <c r="DA13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB13" t="inlineStr">
@@ -18230,7 +18248,7 @@
       </c>
       <c r="DC13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD13" t="inlineStr">
@@ -18240,7 +18258,7 @@
       </c>
       <c r="DE13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF13" t="inlineStr">
@@ -18255,7 +18273,7 @@
       </c>
       <c r="DH13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI13" t="inlineStr">
@@ -18270,7 +18288,7 @@
       </c>
       <c r="DK13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL13" t="inlineStr">
@@ -18280,7 +18298,7 @@
       </c>
       <c r="DM13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN13" t="inlineStr">
@@ -18290,7 +18308,7 @@
       </c>
       <c r="DO13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP13" t="inlineStr">
@@ -18300,7 +18318,7 @@
       </c>
       <c r="DQ13" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR13" t="inlineStr">
@@ -18310,7 +18328,7 @@
       </c>
       <c r="DS13" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT13" t="inlineStr">
@@ -18320,7 +18338,7 @@
       </c>
       <c r="DU13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV13" t="inlineStr">
@@ -18330,7 +18348,7 @@
       </c>
       <c r="DW13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX13" t="inlineStr">
@@ -18340,7 +18358,7 @@
       </c>
       <c r="DY13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ13" t="inlineStr">
@@ -18350,17 +18368,17 @@
       </c>
       <c r="EA13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB13" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED13" t="inlineStr">
@@ -18370,7 +18388,7 @@
       </c>
       <c r="EE13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF13" t="inlineStr">
@@ -18385,7 +18403,7 @@
       </c>
       <c r="EH13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI13" t="inlineStr">
@@ -18400,7 +18418,7 @@
       </c>
       <c r="EK13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL13" t="inlineStr">
@@ -18410,7 +18428,7 @@
       </c>
       <c r="EM13" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN13" t="n">
@@ -18428,7 +18446,7 @@
       </c>
       <c r="EQ13" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER13" t="inlineStr">
@@ -18438,7 +18456,7 @@
       </c>
       <c r="ES13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET13" t="inlineStr">
@@ -18448,7 +18466,7 @@
       </c>
       <c r="EU13" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV13" t="inlineStr">
@@ -18475,22 +18493,24 @@
       <c r="FA13" t="n">
         <v>1</v>
       </c>
-      <c r="FB13" t="n">
-        <v/>
+      <c r="FB13" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC13" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD13" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE13" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF13" t="n">
@@ -18507,7 +18527,7 @@
         </is>
       </c>
       <c r="FI13" t="n">
-        <v/>
+        <v>0.581</v>
       </c>
       <c r="FJ13" t="inlineStr">
         <is>
@@ -18585,22 +18605,22 @@
       </c>
       <c r="FZ13" t="inlineStr">
         <is>
-          <t>degree Celsius</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA13" t="inlineStr">
         <is>
-          <t>µmol s-1 m-2</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB13" t="inlineStr">
         <is>
-          <t>mb</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC13" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -18651,10 +18671,10 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>-169.146333333333</v>
+        <v>-169.14633</v>
       </c>
       <c r="K14" t="n">
-        <v>64.1463333333333</v>
+        <v>64.9915</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
@@ -18952,10 +18972,10 @@
         </is>
       </c>
       <c r="BU14" t="n">
-        <v>28.995</v>
+        <v>28.8</v>
       </c>
       <c r="BV14" t="n">
-        <v/>
+        <v>29.8</v>
       </c>
       <c r="BW14" t="n">
         <v>48</v>
@@ -19029,7 +19049,7 @@
       </c>
       <c r="CM14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN14" t="inlineStr">
@@ -19039,7 +19059,7 @@
       </c>
       <c r="CO14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP14" t="inlineStr">
@@ -19049,7 +19069,7 @@
       </c>
       <c r="CQ14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR14" t="inlineStr">
@@ -19059,7 +19079,7 @@
       </c>
       <c r="CS14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT14" t="n">
@@ -19077,7 +19097,7 @@
       </c>
       <c r="CW14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX14" t="inlineStr">
@@ -19087,7 +19107,7 @@
       </c>
       <c r="CY14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ14" t="inlineStr">
@@ -19097,7 +19117,7 @@
       </c>
       <c r="DA14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB14" t="inlineStr">
@@ -19107,7 +19127,7 @@
       </c>
       <c r="DC14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD14" t="inlineStr">
@@ -19117,7 +19137,7 @@
       </c>
       <c r="DE14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF14" t="inlineStr">
@@ -19132,7 +19152,7 @@
       </c>
       <c r="DH14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI14" t="inlineStr">
@@ -19147,7 +19167,7 @@
       </c>
       <c r="DK14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL14" t="inlineStr">
@@ -19157,7 +19177,7 @@
       </c>
       <c r="DM14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN14" t="inlineStr">
@@ -19167,7 +19187,7 @@
       </c>
       <c r="DO14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP14" t="inlineStr">
@@ -19177,7 +19197,7 @@
       </c>
       <c r="DQ14" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DR14" t="inlineStr">
@@ -19187,7 +19207,7 @@
       </c>
       <c r="DS14" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DT14" t="inlineStr">
@@ -19197,7 +19217,7 @@
       </c>
       <c r="DU14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV14" t="inlineStr">
@@ -19207,7 +19227,7 @@
       </c>
       <c r="DW14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX14" t="inlineStr">
@@ -19217,7 +19237,7 @@
       </c>
       <c r="DY14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ14" t="inlineStr">
@@ -19227,17 +19247,17 @@
       </c>
       <c r="EA14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EB14" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>missing: not collected</t>
         </is>
       </c>
       <c r="EC14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ED14" t="inlineStr">
@@ -19247,7 +19267,7 @@
       </c>
       <c r="EE14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF14" t="inlineStr">
@@ -19262,7 +19282,7 @@
       </c>
       <c r="EH14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI14" t="inlineStr">
@@ -19277,7 +19297,7 @@
       </c>
       <c r="EK14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL14" t="inlineStr">
@@ -19287,7 +19307,7 @@
       </c>
       <c r="EM14" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EN14" t="n">
@@ -19305,7 +19325,7 @@
       </c>
       <c r="EQ14" s="2" t="inlineStr">
         <is>
-          <t>µmol/L</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ER14" t="inlineStr">
@@ -19315,7 +19335,7 @@
       </c>
       <c r="ES14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET14" t="inlineStr">
@@ -19325,7 +19345,7 @@
       </c>
       <c r="EU14" s="2" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV14" t="inlineStr">
@@ -19352,22 +19372,24 @@
       <c r="FA14" t="n">
         <v>1</v>
       </c>
-      <c r="FB14" t="n">
-        <v/>
+      <c r="FB14" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC14" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD14" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE14" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF14" t="n">
@@ -19384,7 +19406,7 @@
         </is>
       </c>
       <c r="FI14" t="n">
-        <v/>
+        <v>0.8279999999999998</v>
       </c>
       <c r="FJ14" t="inlineStr">
         <is>
@@ -19462,22 +19484,22 @@
       </c>
       <c r="FZ14" t="inlineStr">
         <is>
-          <t>degree Celsius</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA14" t="inlineStr">
         <is>
-          <t>µmol s-1 m-2</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB14" t="inlineStr">
         <is>
-          <t>mb</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC14" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -19528,10 +19550,10 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>-169.146333333333</v>
+        <v>-169.14633</v>
       </c>
       <c r="K15" t="n">
-        <v>64.1463333333333</v>
+        <v>64.9915</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -19829,10 +19851,10 @@
         </is>
       </c>
       <c r="BU15" t="n">
-        <v>8.755000000000001</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="BV15" t="n">
-        <v/>
+        <v>9.699999999999999</v>
       </c>
       <c r="BW15" t="n">
         <v>48</v>
@@ -19904,7 +19926,7 @@
       </c>
       <c r="CM15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CN15" t="inlineStr">
@@ -19914,7 +19936,7 @@
       </c>
       <c r="CO15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CP15" t="inlineStr">
@@ -19924,7 +19946,7 @@
       </c>
       <c r="CQ15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CR15" t="inlineStr">
@@ -19934,7 +19956,7 @@
       </c>
       <c r="CS15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CT15" t="n">
@@ -19952,7 +19974,7 @@
       </c>
       <c r="CW15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CX15" t="inlineStr">
@@ -19962,7 +19984,7 @@
       </c>
       <c r="CY15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="CZ15" t="inlineStr">
@@ -19972,7 +19994,7 @@
       </c>
       <c r="DA15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DB15" t="inlineStr">
@@ -19982,7 +20004,7 @@
       </c>
       <c r="DC15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DD15" t="inlineStr">
@@ -19992,7 +20014,7 @@
       </c>
       <c r="DE15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DF15" t="inlineStr">
@@ -20007,7 +20029,7 @@
       </c>
       <c r="DH15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DI15" t="inlineStr">
@@ -20022,7 +20044,7 @@
       </c>
       <c r="DK15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DL15" t="inlineStr">
@@ -20032,7 +20054,7 @@
       </c>
       <c r="DM15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DN15" t="inlineStr">
@@ -20042,7 +20064,7 @@
       </c>
       <c r="DO15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DP15" t="n">
@@ -20068,7 +20090,7 @@
       </c>
       <c r="DU15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DV15" t="inlineStr">
@@ -20078,7 +20100,7 @@
       </c>
       <c r="DW15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DX15" t="inlineStr">
@@ -20088,7 +20110,7 @@
       </c>
       <c r="DY15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="DZ15" t="inlineStr">
@@ -20098,17 +20120,17 @@
       </c>
       <c r="EA15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
-        </is>
-      </c>
-      <c r="EB15" t="inlineStr">
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EB15" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="EC15" t="inlineStr">
         <is>
           <t>µmol/L</t>
         </is>
       </c>
-      <c r="EC15" t="n">
-        <v>0.57</v>
-      </c>
       <c r="ED15" t="inlineStr">
         <is>
           <t>missing: not collected</t>
@@ -20116,7 +20138,7 @@
       </c>
       <c r="EE15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EF15" t="inlineStr">
@@ -20131,7 +20153,7 @@
       </c>
       <c r="EH15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EI15" t="inlineStr">
@@ -20146,7 +20168,7 @@
       </c>
       <c r="EK15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EL15" t="n">
@@ -20180,7 +20202,7 @@
       </c>
       <c r="ES15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="ET15" t="inlineStr">
@@ -20190,7 +20212,7 @@
       </c>
       <c r="EU15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="EV15" t="inlineStr">
@@ -20217,22 +20239,24 @@
       <c r="FA15" t="n">
         <v>1</v>
       </c>
-      <c r="FB15" t="n">
-        <v/>
+      <c r="FB15" t="inlineStr">
+        <is>
+          <t>AlaskaArctic22-23_extSet_2</t>
+        </is>
       </c>
       <c r="FC15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FD15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FE15" t="inlineStr">
         <is>
-          <t>missing: not collected</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FF15" t="n">
@@ -20249,7 +20273,7 @@
         </is>
       </c>
       <c r="FI15" t="n">
-        <v/>
+        <v>1.38</v>
       </c>
       <c r="FJ15" t="inlineStr">
         <is>
@@ -20326,7 +20350,7 @@
       </c>
       <c r="GC15" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
         </is>
       </c>
     </row>
@@ -20779,472 +20803,472 @@
       </c>
       <c r="CM16" t="inlineStr">
         <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="CN16" t="inlineStr">
+        <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CN16" t="inlineStr">
+      <c r="CO16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="CP16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CO16" t="inlineStr">
+      <c r="CQ16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="CR16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CP16" t="inlineStr">
+      <c r="CS16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="CT16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CQ16" t="inlineStr">
+      <c r="CU16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="CV16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CR16" t="inlineStr">
+      <c r="CW16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="CX16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CS16" t="inlineStr">
+      <c r="CY16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="CZ16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CT16" t="inlineStr">
+      <c r="DA16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DB16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CU16" t="inlineStr">
+      <c r="DC16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DD16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CV16" t="inlineStr">
+      <c r="DE16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DF16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CW16" t="inlineStr">
+      <c r="DG16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CX16" t="inlineStr">
+      <c r="DH16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DI16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CY16" t="inlineStr">
+      <c r="DJ16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="CZ16" t="inlineStr">
+      <c r="DK16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DL16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DA16" t="inlineStr">
+      <c r="DM16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DN16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DB16" t="inlineStr">
+      <c r="DO16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DP16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DC16" t="inlineStr">
+      <c r="DQ16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DR16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DD16" t="inlineStr">
+      <c r="DS16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DT16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DE16" t="inlineStr">
+      <c r="DU16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DV16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DF16" t="inlineStr">
+      <c r="DW16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DX16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DG16" t="inlineStr">
+      <c r="DY16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="DZ16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DH16" t="inlineStr">
+      <c r="EA16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EB16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DI16" t="inlineStr">
+      <c r="EC16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="ED16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DJ16" t="inlineStr">
+      <c r="EE16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EF16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DK16" t="inlineStr">
+      <c r="EG16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DL16" t="inlineStr">
+      <c r="EH16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EI16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DM16" t="inlineStr">
+      <c r="EJ16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DN16" t="inlineStr">
+      <c r="EK16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EL16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DO16" t="inlineStr">
+      <c r="EM16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EN16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DP16" t="inlineStr">
+      <c r="EO16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EP16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DQ16" t="inlineStr">
+      <c r="EQ16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="ER16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DR16" t="inlineStr">
+      <c r="ES16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="ET16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DS16" t="inlineStr">
+      <c r="EU16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="EV16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DT16" t="inlineStr">
+      <c r="EW16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DU16" t="inlineStr">
+      <c r="EX16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DV16" t="inlineStr">
+      <c r="EY16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DW16" t="inlineStr">
+      <c r="EZ16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DX16" t="inlineStr">
+      <c r="FA16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DY16" t="inlineStr">
+      <c r="FB16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="DZ16" t="inlineStr">
+      <c r="FC16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EA16" t="inlineStr">
+      <c r="FD16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EB16" t="inlineStr">
+      <c r="FE16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EC16" t="inlineStr">
+      <c r="FF16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="ED16" t="inlineStr">
+      <c r="FG16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EE16" t="inlineStr">
+      <c r="FH16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EF16" t="inlineStr">
+      <c r="FI16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EG16" t="inlineStr">
+      <c r="FJ16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
+      <c r="FK16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EH16" t="inlineStr">
+      <c r="FL16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EI16" t="inlineStr">
+      <c r="FM16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EJ16" t="inlineStr">
+      <c r="FN16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EK16" t="inlineStr">
+      <c r="FO16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EL16" t="inlineStr">
+      <c r="FP16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EM16" t="inlineStr">
+      <c r="FQ16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EN16" t="inlineStr">
+      <c r="FR16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EO16" t="inlineStr">
+      <c r="FS16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EP16" t="inlineStr">
+      <c r="FT16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EQ16" t="inlineStr">
+      <c r="FU16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="ER16" t="inlineStr">
+      <c r="FV16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="ES16" t="inlineStr">
+      <c r="FW16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="ET16" t="inlineStr">
+      <c r="FX16" t="inlineStr">
         <is>
           <t>not applicable: control sample</t>
         </is>
       </c>
-      <c r="EU16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="EV16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="EW16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="EX16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="EY16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="EZ16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FA16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FB16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FC16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FD16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FE16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FF16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FG16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FH16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FI16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FJ16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FK16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FL16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FM16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FN16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FO16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FP16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FQ16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FR16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FS16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FT16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FU16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FV16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FW16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
-      <c r="FX16" t="inlineStr">
-        <is>
-          <t>not applicable: control sample</t>
-        </is>
-      </c>
       <c r="FY16" t="inlineStr">
         <is>
-          <t>not applicable: control sample</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="FZ16" t="inlineStr">
         <is>
-          <t>not applicable: control sample</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GA16" t="inlineStr">
         <is>
-          <t>not applicable: control sample</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GB16" t="inlineStr">
         <is>
-          <t>not applicable: control sample</t>
+          <t>not applicable</t>
         </is>
       </c>
       <c r="GC16" t="inlineStr">

</xml_diff>

<commit_message>
finalize sampleMetadata for 2306
</commit_message>
<xml_diff>
--- a/projects/EcoFoci/dy2209/data/dy2209_faire.xlsx
+++ b/projects/EcoFoci/dy2209/data/dy2209_faire.xlsx
@@ -10220,10 +10220,10 @@
         </is>
       </c>
       <c r="BU4" s="2" t="n">
-        <v>32</v>
+        <v>31.92</v>
       </c>
       <c r="BV4" s="2" t="n">
-        <v>33</v>
+        <v>32.92</v>
       </c>
       <c r="BW4" s="2" t="n">
         <v>18</v>
@@ -10747,7 +10747,7 @@
       </c>
       <c r="GC4" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -11101,10 +11101,10 @@
         </is>
       </c>
       <c r="BU5" t="n">
-        <v>19.4</v>
+        <v>19.32</v>
       </c>
       <c r="BV5" t="n">
-        <v>20.4</v>
+        <v>20.32</v>
       </c>
       <c r="BW5" t="n">
         <v>18</v>
@@ -11628,7 +11628,7 @@
       </c>
       <c r="GC5" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -11982,10 +11982,10 @@
         </is>
       </c>
       <c r="BU6" t="n">
-        <v>8.699999999999999</v>
+        <v>8.710000000000001</v>
       </c>
       <c r="BV6" t="n">
-        <v>9.699999999999999</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="BW6" t="n">
         <v>18</v>
@@ -12509,7 +12509,7 @@
       </c>
       <c r="GC6" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -12863,10 +12863,10 @@
         </is>
       </c>
       <c r="BU7" t="n">
-        <v>32.7</v>
+        <v>32.55</v>
       </c>
       <c r="BV7" t="n">
-        <v>33.7</v>
+        <v>33.55</v>
       </c>
       <c r="BW7" t="n">
         <v>37</v>
@@ -13390,7 +13390,7 @@
       </c>
       <c r="GC7" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -13744,10 +13744,10 @@
         </is>
       </c>
       <c r="BU8" t="n">
-        <v>18.8</v>
+        <v>18.69</v>
       </c>
       <c r="BV8" t="n">
-        <v>19.8</v>
+        <v>19.69</v>
       </c>
       <c r="BW8" t="n">
         <v>37</v>
@@ -14271,7 +14271,7 @@
       </c>
       <c r="GC8" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -14625,10 +14625,10 @@
         </is>
       </c>
       <c r="BU9" t="n">
-        <v>8.300000000000001</v>
+        <v>8.25</v>
       </c>
       <c r="BV9" t="n">
-        <v>9.300000000000001</v>
+        <v>9.25</v>
       </c>
       <c r="BW9" t="n">
         <v>37</v>
@@ -15152,7 +15152,7 @@
       </c>
       <c r="GC9" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -15506,10 +15506,10 @@
         </is>
       </c>
       <c r="BU10" t="n">
-        <v>40.4</v>
+        <v>40.26</v>
       </c>
       <c r="BV10" t="n">
-        <v>41.4</v>
+        <v>41.26</v>
       </c>
       <c r="BW10" t="n">
         <v>45</v>
@@ -16025,7 +16025,7 @@
       </c>
       <c r="GC10" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -16379,10 +16379,10 @@
         </is>
       </c>
       <c r="BU11" t="n">
-        <v>28.5</v>
+        <v>28.44</v>
       </c>
       <c r="BV11" t="n">
-        <v>29.5</v>
+        <v>29.44</v>
       </c>
       <c r="BW11" t="n">
         <v>45</v>
@@ -16878,7 +16878,7 @@
       </c>
       <c r="GC11" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -17741,7 +17741,7 @@
       </c>
       <c r="GC12" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -18093,10 +18093,10 @@
         </is>
       </c>
       <c r="BU13" t="n">
-        <v>42.3</v>
+        <v>42.14</v>
       </c>
       <c r="BV13" t="n">
-        <v>43.3</v>
+        <v>43.14</v>
       </c>
       <c r="BW13" t="n">
         <v>48</v>
@@ -18620,7 +18620,7 @@
       </c>
       <c r="GC13" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -18972,10 +18972,10 @@
         </is>
       </c>
       <c r="BU14" t="n">
-        <v>28.8</v>
+        <v>28.7</v>
       </c>
       <c r="BV14" t="n">
-        <v>29.8</v>
+        <v>29.7</v>
       </c>
       <c r="BW14" t="n">
         <v>48</v>
@@ -19499,7 +19499,7 @@
       </c>
       <c r="GC14" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>
@@ -19851,10 +19851,10 @@
         </is>
       </c>
       <c r="BU15" t="n">
-        <v>8.699999999999999</v>
+        <v>8.66</v>
       </c>
       <c r="BV15" t="n">
-        <v>9.699999999999999</v>
+        <v>9.66</v>
       </c>
       <c r="BW15" t="n">
         <v>48</v>
@@ -20350,7 +20350,7 @@
       </c>
       <c r="GC15" t="inlineStr">
         <is>
-          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file.</t>
+          <t>All measurement metadata reported for this sample are taken from a mix of the CTD data file and the bottle file. par, air_pressure_at_sea_level, wind_direction, wind_speed, air_temperature, silicate, nitrate, nitrite, phosphate, and ammonium are reported from the CTD data file. latitude, longitude, chorophyll, percent_oxygen_sat, diss_oxygen, salinity, density, temp, pressure, and turbidity are reported from the bottle file. Depth was calculated from pressure.</t>
         </is>
       </c>
     </row>

</xml_diff>